<commit_message>
example has an extra column
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/GeneticsFile.xlsx
+++ b/doc/Manual/Batchmode/GeneticsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D7128A-7143-4C32-BBEC-986AA7224FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6DB82F-180F-499F-BEF0-0521FBD171F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Simulation</t>
   </si>
@@ -596,21 +596,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="67.28515625" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
+    <col min="3" max="3" width="52.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -621,7 +621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -632,7 +632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -643,7 +643,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -654,7 +654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -665,7 +665,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -676,7 +676,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -687,7 +687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -698,7 +698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -709,7 +709,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -720,7 +720,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -731,7 +731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -742,7 +742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -753,7 +753,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -764,97 +764,97 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C27"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C28"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C29"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C30"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C31"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C32"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45"/>
     </row>
   </sheetData>
@@ -864,26 +864,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -897,37 +896,34 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -949,29 +945,26 @@
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2">
-        <v>3</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -985,33 +978,30 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="F3" t="b">
+      <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="G3" t="b">
+      <c r="H3">
         <v>0</v>
       </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
       <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
         <v>2</v>
       </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
       <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
         <v>14</v>
       </c>
-      <c r="M3">
+      <c r="L3">
         <v>10</v>
       </c>
-      <c r="N3" t="s">
+      <c r="M3" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
precision on chromosome ends
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/GeneticsFile.xlsx
+++ b/doc/Manual/Batchmode/GeneticsFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6DB82F-180F-499F-BEF0-0521FBD171F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28CDEAF-48FF-4308-B046-41411F4D977C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1032" windowWidth="21600" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>Simulation</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Comma separated list of integers, or # to leave empty</t>
-  </si>
-  <si>
-    <t>Recombination rate (through chromosomal crossover) across the whole genome (in addition to the chromosomeEnds above).</t>
   </si>
   <si>
     <t>TRUE/FALSE</t>
@@ -159,7 +156,13 @@
     <t>Single integer value &gt; 0, &lt; GenomeSize</t>
   </si>
   <si>
-    <t>Where the genome is split into chromosomes. Note that positions go from 0 to GenomeSize - 1. If empty, a single chromosome is created. These areas recombine with a probability of 0.5.</t>
+    <t>Where the genome is split into chromosomes. Note that positions go from 0 to GenomeSize - 1. If empty, a single chromosome is created. These areas recombine with a probability of 0.5. Disabled for haploid organisms (no recombination).</t>
+  </si>
+  <si>
+    <t>Recombination rate (through chromosomal crossover) across the whole genome (in addition to the chromosomeEnds above). Disabled for haploid organisms (no recombination).</t>
+  </si>
+  <si>
+    <t>Comma separated list of integers, or # to leave empty. Must be # for haploid (asexual) systems.</t>
   </si>
 </sst>
 </file>
@@ -596,21 +599,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="67.33203125" customWidth="1"/>
-    <col min="3" max="3" width="52.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="67.28515625" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -618,21 +621,21 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -640,221 +643,221 @@
         <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:3" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:3" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45"/>
     </row>
   </sheetData>
@@ -866,23 +869,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -899,10 +902,10 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
         <v>36</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -923,7 +926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -964,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
comma-separated lists in input replaced with semicolon-separated lists
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/GeneticsFile.xlsx
+++ b/doc/Manual/Batchmode/GeneticsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9FFB82-B2ED-46F5-8E4C-67C028D54CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9723152-EB43-44A9-8554-3FD79E27FA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2400" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -68,15 +68,6 @@
     <t>random</t>
   </si>
   <si>
-    <t>5, 10, 15</t>
-  </si>
-  <si>
-    <t>4,5,8</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
     <t>Single integer value</t>
   </si>
   <si>
@@ -114,12 +105,6 @@
     <t>Positive integer if any output is TRUE, otherwise either 0 or #.</t>
   </si>
   <si>
-    <t>Either 1) comma-separated list (CSL), 2) ‘random’, 3) ‘random_occupied’ or 4) ‘all’. Patch 0 is reserved for an internal matrix and cannot be selected (if the CSL option is chosen). In the CSL and random case, there is no internal check of whether the specified/sampled patch exist through the simulation, so it is up to the user to ensure this is the case, and special care should be given for dynamic landscapes.</t>
-  </si>
-  <si>
-    <t>Comma-separated list or "all"</t>
-  </si>
-  <si>
     <t>Which patches are to be sampled for output.  Patches can be specified according to their patch number, as per the patch layer in a patch-based model. Or sampled randomly or all patches can be chosen. In a cell-based landscape random is the only option with number of patches (=cells) specified.</t>
   </si>
   <si>
@@ -156,7 +141,22 @@
     <t>Recombination rate (through chromosomal crossover) across the whole genome (in addition to the chromosomeEnds above). Disabled for haploid organisms (no recombination).</t>
   </si>
   <si>
-    <t>Comma separated list of integers, or # to leave empty. Must be # for haploid (asexual) systems.</t>
+    <t>5;10;15</t>
+  </si>
+  <si>
+    <t>4;5;8</t>
+  </si>
+  <si>
+    <t>1;2</t>
+  </si>
+  <si>
+    <t>Semicolon separated list of integers, or # to leave empty. Must be # for haploid (asexual) systems.</t>
+  </si>
+  <si>
+    <t>Either 1) Semicolon-separated list (CSL), 2) ‘random’, 3) ‘random_occupied’ or 4) ‘all’. Patch 0 is reserved for an internal matrix and cannot be selected (if the CSL option is chosen). In the CSL and random case, there is no internal check of whether the specified/sampled patch exist through the simulation, so it is up to the user to ensure this is the case, and special care should be given for dynamic landscapes.</t>
+  </si>
+  <si>
+    <t>Semicolon-separated list or "all"</t>
   </si>
 </sst>
 </file>
@@ -593,21 +593,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="67.33203125" customWidth="1"/>
-    <col min="3" max="3" width="52.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="67.28515625" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -615,243 +615,243 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45"/>
     </row>
   </sheetData>
@@ -863,23 +863,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -896,10 +896,10 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -920,7 +920,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -969,7 +969,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>5.0000000000000001E-3</v>
@@ -990,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
         <v>13</v>
@@ -999,7 +999,7 @@
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>